<commit_message>
Lab4 Added 'const' to some functions signatures. Added a new test case in 'test_cases.xlsx'
</commit_message>
<xml_diff>
--- a/Lab4/test_cases.xlsx
+++ b/Lab4/test_cases.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\gwscistud.gmadtree.gmit.ie\STUD\G00329649\Documents\OS\OS\Lab4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\Documents\OS\OS\Lab4\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="4">
   <si>
     <t>P1</t>
   </si>
@@ -353,23 +353,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:G12"/>
+  <dimension ref="B2:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>3</v>
       </c>
       <c r="E2">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -379,16 +382,22 @@
       <c r="F3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>10</v>
       </c>
       <c r="E4">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>1</v>
       </c>
@@ -399,16 +408,22 @@
         <f>E4</f>
         <v>21</v>
       </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>5</v>
       </c>
       <c r="E6">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I6">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>2</v>
       </c>
@@ -419,16 +434,22 @@
         <f>E4+E6</f>
         <v>24</v>
       </c>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>7</v>
       </c>
       <c r="E8">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E9" t="s">
         <v>3</v>
       </c>
@@ -436,13 +457,19 @@
         <f>E4+E6+E8</f>
         <v>30</v>
       </c>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E10">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E11">
         <v>1</v>
       </c>
@@ -454,10 +481,26 @@
         <f>F11/COUNT(F3:F10)</f>
         <v>18.75</v>
       </c>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E12">
         <v>2</v>
+      </c>
+      <c r="I12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E14">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>